<commit_message>
fixed across-host pi values, slides for meeting.
</commit_message>
<xml_diff>
--- a/HMP1-2_oral_file_manifest_sample_ordered.xlsx
+++ b/HMP1-2_oral_file_manifest_sample_ordered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5261b2f2f3e51194/Desktop/GitHub/demo_for_ccgb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="13_ncr:40009_{CBA161DB-F2C7-4F07-B72D-33F021730ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA9C2086-6303-41EC-90E7-CFD703ED2C9F}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:40009_{CBA161DB-F2C7-4F07-B72D-33F021730ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E8CC1D3-ECF7-439C-90E0-F2FF3922C026}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="2580" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5640" yWindow="3180" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HMP1-2_oral_file_manifest_sampl" sheetId="1" r:id="rId1"/>
@@ -6521,8 +6521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6530,7 +6530,7 @@
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="102.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.140625" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -15482,7 +15482,7 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G380">
-      <sortCondition ref="E1"/>
+      <sortCondition ref="G1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>